<commit_message>
Adds new checklist versions. Adds reference to MASVS V5.2 in 0x4f.
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-English_1.1.0.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-English_1.1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mitm/git-repos/owasp-mstg/Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D4CD9B-7B0B-7C49-95A1-3AFB57E83568}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2B6841-07AC-3340-98FD-EC00A82B2165}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4200" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8789,8 +8789,8 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>